<commit_message>
gai goth complete and estimate of subodh sir complete
</commit_message>
<xml_diff>
--- a/ofc/estimates/nagar aspatal emergency ward/estimate (1).xlsx
+++ b/ofc/estimates/nagar aspatal emergency ward/estimate (1).xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\nagar aspatal emergency ward\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\nagar aspatal emergency ward\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7452"/>
   </bookViews>
   <sheets>
     <sheet name="estimate (2)" sheetId="25" r:id="rId1"/>
@@ -119,7 +119,7 @@
     <definedName name="Ttile">'[1]update Rate'!$N$43</definedName>
     <definedName name="unskilled">'[2]Material rate'!$D$154</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -313,10 +313,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -498,7 +498,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="95">
@@ -509,7 +509,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,14 +529,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,7 +545,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -566,7 +566,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,7 +592,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -605,7 +605,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -618,7 +618,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -637,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,13 +678,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,6 +703,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -722,21 +737,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1589,25 +1589,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
@@ -1622,7 +1622,7 @@
       <c r="J1" s="77"/>
       <c r="K1" s="77"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="J2" s="78"/>
       <c r="K2" s="78"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="J4" s="79"/>
       <c r="K4" s="79"/>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +1682,7 @@
       <c r="J5" s="80"/>
       <c r="K5" s="80"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="81" t="s">
         <v>47</v>
       </c>
@@ -1699,24 +1699,24 @@
       <c r="J6" s="82"/>
       <c r="K6" s="82"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="M8" s="31"/>
     </row>
-    <row r="9" spans="1:13" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -1780,7 +1780,7 @@
       <c r="K9" s="21"/>
       <c r="M9" s="70"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="55"/>
       <c r="B10" s="59" t="s">
         <v>43</v>
@@ -1809,7 +1809,7 @@
       <c r="K10" s="56"/>
       <c r="M10" s="70"/>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="55"/>
       <c r="B11" s="59" t="s">
         <v>42</v>
@@ -1838,7 +1838,7 @@
       <c r="K11" s="56"/>
       <c r="M11" s="61"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="55"/>
       <c r="B12" s="59" t="s">
         <v>41</v>
@@ -1866,7 +1866,7 @@
       <c r="J12" s="58"/>
       <c r="K12" s="56"/>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="33" t="s">
         <v>31</v>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="33"/>
       <c r="C14" s="19"/>
@@ -1905,7 +1905,7 @@
       <c r="J14" s="36"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -1922,7 +1922,7 @@
       <c r="J15" s="30"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="55"/>
       <c r="B16" s="59" t="s">
         <v>44</v>
@@ -1939,21 +1939,21 @@
         <v>1.8</v>
       </c>
       <c r="G16" s="60">
-        <f>F16</f>
-        <v>1.8</v>
+        <f>PRODUCT(C16:F16)</f>
+        <v>10.012191405059433</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
       <c r="J16" s="58"/>
       <c r="K16" s="56"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="55"/>
       <c r="B17" s="59" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D17" s="12">
         <v>0.874</v>
@@ -1963,15 +1963,15 @@
         <v>1.8</v>
       </c>
       <c r="G17" s="60">
-        <f t="shared" ref="G17:G18" si="2">F17</f>
-        <v>1.8</v>
+        <f t="shared" ref="G17:G18" si="2">PRODUCT(C17:F17)</f>
+        <v>-1.5731999999999999</v>
       </c>
       <c r="H17" s="58"/>
       <c r="I17" s="58"/>
       <c r="J17" s="58"/>
       <c r="K17" s="56"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55"/>
       <c r="B18" s="59" t="s">
         <v>46</v>
@@ -1984,18 +1984,18 @@
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12">
-        <v>1.78</v>
+        <v>1.8</v>
       </c>
       <c r="G18" s="60">
         <f t="shared" si="2"/>
-        <v>1.78</v>
+        <v>1.8360000000000001</v>
       </c>
       <c r="H18" s="58"/>
       <c r="I18" s="58"/>
       <c r="J18" s="58"/>
       <c r="K18" s="56"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="33" t="s">
         <v>31</v>
@@ -2006,35 +2006,35 @@
       <c r="F19" s="21"/>
       <c r="G19" s="23">
         <f>SUM(G16:G18)</f>
-        <v>5.38</v>
+        <v>10.274991405059433</v>
       </c>
       <c r="H19" s="22" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="23">
-        <f>5476.83*1.15</f>
-        <v>6298.3544999999995</v>
+        <f>4465.4*1.15</f>
+        <v>5135.2099999999991</v>
       </c>
       <c r="J19" s="36">
         <f>G19*I19</f>
-        <v>33885.147209999996</v>
+        <v>52764.238613175243</v>
       </c>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
-      <c r="B20" s="28"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
-      <c r="G20" s="30"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="22"/>
       <c r="I20" s="23"/>
-      <c r="J20" s="30"/>
+      <c r="J20" s="36"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="37" t="s">
         <v>16</v>
@@ -2047,12 +2047,12 @@
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
       <c r="J21" s="36">
-        <f>SUM(J9:J20)</f>
-        <v>46326.255556332209</v>
+        <f>SUM(J9:J19)</f>
+        <v>65205.346959507457</v>
       </c>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="46"/>
       <c r="B22" s="49"/>
       <c r="C22" s="50"/>
@@ -2065,16 +2065,16 @@
       <c r="J22" s="48"/>
       <c r="K22" s="45"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
       <c r="B23" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="76">
+      <c r="C23" s="74">
         <f>J21</f>
-        <v>46326.255556332209</v>
-      </c>
-      <c r="D23" s="76"/>
+        <v>65205.346959507457</v>
+      </c>
+      <c r="D23" s="74"/>
       <c r="E23" s="40"/>
       <c r="F23" s="41"/>
       <c r="G23" s="40"/>
@@ -2082,16 +2082,16 @@
       <c r="I23" s="43"/>
       <c r="J23" s="44"/>
     </row>
-    <row r="24" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="45"/>
       <c r="B24" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="76">
+      <c r="C24" s="74">
         <f>0.13*C23</f>
-        <v>6022.4132223231873</v>
-      </c>
-      <c r="D24" s="76"/>
+        <v>8476.6951047359689</v>
+      </c>
+      <c r="D24" s="74"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45"/>
       <c r="G24" s="45"/>
@@ -2099,85 +2099,85 @@
       <c r="I24" s="45"/>
       <c r="J24" s="45"/>
     </row>
-    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="76">
+      <c r="C25" s="74">
         <f>SUM(C23:D24)</f>
-        <v>52348.668778655396</v>
-      </c>
-      <c r="D25" s="76"/>
-    </row>
-    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>73682.042064243433</v>
+      </c>
+      <c r="D25" s="74"/>
+    </row>
+    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
@@ -2191,60 +2191,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="62" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-    </row>
-    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="93" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:16" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="K3" s="79"/>
       <c r="N3" s="64"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
@@ -2276,31 +2276,31 @@
       <c r="K4" s="79"/>
       <c r="N4" s="64"/>
     </row>
-    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="94" t="s">
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="90">
+      <c r="C6" s="83">
         <f>F17</f>
-        <v>46326.255556332209</v>
-      </c>
-      <c r="D6" s="91"/>
+        <v>65205.346959507457</v>
+      </c>
+      <c r="D6" s="84"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2308,28 +2308,28 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="90">
+      <c r="J6" s="83">
         <f>I17</f>
-        <v>46326.255556332209</v>
-      </c>
-      <c r="K6" s="91"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>65100.588675507453</v>
+      </c>
+      <c r="K6" s="84"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="I7" s="86" t="s">
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="I7" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="81" t="str">
         <f>Valuated!A6</f>
         <v>Project:- नगर अस्पताल मर्मत</v>
@@ -2339,59 +2339,59 @@
       <c r="D8" s="81"/>
       <c r="E8" s="81"/>
       <c r="F8" s="81"/>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="88" t="str">
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="93" t="str">
         <f>Valuated!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="I9" s="87" t="s">
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="I9" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="87"/>
-      <c r="K9" s="87"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="83" t="s">
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="89" t="s">
+      <c r="D11" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89" t="s">
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="83" t="s">
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="89" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2410,10 +2410,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="83"/>
-      <c r="K12" s="84"/>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J12" s="88"/>
+      <c r="K12" s="89"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <f>'estimate (2)'!A9</f>
         <v>1</v>
@@ -2459,7 +2459,7 @@
       <c r="O13" s="66"/>
       <c r="P13" s="66"/>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="27"/>
       <c r="C14" s="12"/>
@@ -2475,7 +2475,7 @@
       <c r="O14" s="66"/>
       <c r="P14" s="66"/>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <f>'estimate (2)'!A15</f>
         <v>2</v>
@@ -2490,38 +2490,38 @@
       </c>
       <c r="D15" s="12">
         <f>'estimate (2)'!G19</f>
-        <v>5.38</v>
+        <v>10.274991405059433</v>
       </c>
       <c r="E15" s="12">
         <f>'estimate (2)'!I19</f>
-        <v>6298.3544999999995</v>
+        <v>5135.2099999999991</v>
       </c>
       <c r="F15" s="12">
         <f>D15*E15</f>
-        <v>33885.147209999996</v>
+        <v>52764.238613175243</v>
       </c>
       <c r="G15" s="12">
         <f>Valuated!G19</f>
-        <v>5.38</v>
+        <v>10.254591405059433</v>
       </c>
       <c r="H15" s="12">
         <f>Valuated!I19</f>
-        <v>6298.3544999999995</v>
+        <v>5135.2099999999991</v>
       </c>
       <c r="I15" s="12">
         <f>G15*H15</f>
-        <v>33885.147209999996</v>
+        <v>52659.48032917524</v>
       </c>
       <c r="J15" s="26">
         <f>I15-F15</f>
-        <v>0</v>
+        <v>-104.75828400000319</v>
       </c>
       <c r="K15" s="14"/>
       <c r="N15" s="64"/>
       <c r="O15" s="66"/>
       <c r="P15" s="66"/>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
       <c r="B16" s="27"/>
       <c r="C16" s="12"/>
@@ -2537,7 +2537,7 @@
       <c r="O16" s="66"/>
       <c r="P16" s="66"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -2547,23 +2547,23 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7">
         <f>SUM(F13:F15)</f>
-        <v>46326.255556332209</v>
+        <v>65205.346959507457</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7">
         <f>SUM(I13:I15)</f>
-        <v>46326.255556332209</v>
+        <v>65100.588675507453</v>
       </c>
       <c r="J17" s="13">
         <f>I17-F17</f>
-        <v>0</v>
+        <v>-104.75828400000319</v>
       </c>
       <c r="K17" s="5"/>
       <c r="O17" s="65"/>
       <c r="P17" s="66"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>55</v>
@@ -2573,23 +2573,23 @@
       <c r="E18" s="67"/>
       <c r="F18" s="7">
         <f>0.13*F17</f>
-        <v>6022.4132223231873</v>
+        <v>8476.6951047359689</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7">
         <f>0.13*I17</f>
-        <v>6022.4132223231873</v>
+        <v>8463.0765278159688</v>
       </c>
       <c r="J18" s="13">
         <f t="shared" ref="J18:J19" si="3">I18-F18</f>
-        <v>0</v>
+        <v>-13.618576920000123</v>
       </c>
       <c r="K18" s="5"/>
       <c r="O18" s="65"/>
       <c r="P18" s="66"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
         <v>56</v>
@@ -2599,75 +2599,68 @@
       <c r="E19" s="67"/>
       <c r="F19" s="7">
         <f>SUM(F17:F18)</f>
-        <v>52348.668778655396</v>
+        <v>73682.042064243433</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7">
         <f>SUM(I17:I18)</f>
-        <v>52348.668778655396</v>
+        <v>73563.665203323428</v>
       </c>
       <c r="J19" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-118.37686092000513</v>
       </c>
       <c r="K19" s="5"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O20" s="65"/>
       <c r="P20" s="66"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O21" s="65"/>
       <c r="P21" s="66"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O22" s="65"/>
       <c r="P22" s="66"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O23" s="65"/>
       <c r="P23" s="66"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="N24" s="51"/>
       <c r="O24" s="65"/>
       <c r="P24" s="66"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O25" s="65"/>
       <c r="P25" s="65"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="N26" s="63"/>
       <c r="O26" s="65"/>
       <c r="P26" s="65"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="N28" s="67"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="N29" s="67"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O30" s="65"/>
       <c r="P30" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2681,6 +2674,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2698,25 +2698,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="J1" s="77"/>
       <c r="K1" s="77"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="J2" s="78"/>
       <c r="K2" s="78"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="J4" s="79"/>
       <c r="K4" s="79"/>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
         <v>49</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="J5" s="80"/>
       <c r="K5" s="80"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="81" t="s">
         <v>47</v>
       </c>
@@ -2808,24 +2808,24 @@
       <c r="J6" s="82"/>
       <c r="K6" s="82"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="M8" s="31"/>
     </row>
-    <row r="9" spans="1:13" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="K9" s="21"/>
       <c r="M9" s="70"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="55"/>
       <c r="B10" s="59" t="s">
         <v>43</v>
@@ -2905,11 +2905,11 @@
         <v>0.70599999999999996</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" ref="F10:F11" si="0">PRODUCT(C10:E10)</f>
+        <f>PRODUCT(C10:E10)</f>
         <v>5.5946357817738486</v>
       </c>
       <c r="G10" s="60">
-        <f t="shared" ref="G10:G11" si="1">F10</f>
+        <f>F10</f>
         <v>5.5946357817738486</v>
       </c>
       <c r="H10" s="58"/>
@@ -2918,7 +2918,7 @@
       <c r="K10" s="56"/>
       <c r="M10" s="70"/>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="55"/>
       <c r="B11" s="59" t="s">
         <v>42</v>
@@ -2934,11 +2934,11 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F10:F11" si="0">PRODUCT(C11:E11)</f>
         <v>30.726328964746518</v>
       </c>
       <c r="G11" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G10:G11" si="1">F11</f>
         <v>30.726328964746518</v>
       </c>
       <c r="H11" s="58"/>
@@ -2947,7 +2947,7 @@
       <c r="K11" s="56"/>
       <c r="M11" s="61"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="55"/>
       <c r="B12" s="59" t="s">
         <v>41</v>
@@ -2975,7 +2975,7 @@
       <c r="J12" s="58"/>
       <c r="K12" s="56"/>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="33" t="s">
         <v>31</v>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="33"/>
       <c r="C14" s="19"/>
@@ -3014,7 +3014,7 @@
       <c r="J14" s="36"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -3031,7 +3031,7 @@
       <c r="J15" s="30"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="55"/>
       <c r="B16" s="59" t="s">
         <v>44</v>
@@ -3048,21 +3048,21 @@
         <v>1.8</v>
       </c>
       <c r="G16" s="60">
-        <f>F16</f>
-        <v>1.8</v>
+        <f>PRODUCT(C16:F16)</f>
+        <v>10.012191405059433</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
       <c r="J16" s="58"/>
       <c r="K16" s="56"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="55"/>
       <c r="B17" s="59" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D17" s="12">
         <v>0.874</v>
@@ -3072,15 +3072,15 @@
         <v>1.8</v>
       </c>
       <c r="G17" s="60">
-        <f t="shared" ref="G17:G18" si="2">F17</f>
-        <v>1.8</v>
+        <f t="shared" ref="G17:G18" si="2">PRODUCT(C17:F17)</f>
+        <v>-1.5731999999999999</v>
       </c>
       <c r="H17" s="58"/>
       <c r="I17" s="58"/>
       <c r="J17" s="58"/>
       <c r="K17" s="56"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55"/>
       <c r="B18" s="59" t="s">
         <v>46</v>
@@ -3097,14 +3097,14 @@
       </c>
       <c r="G18" s="60">
         <f t="shared" si="2"/>
-        <v>1.78</v>
+        <v>1.8156000000000001</v>
       </c>
       <c r="H18" s="58"/>
       <c r="I18" s="58"/>
       <c r="J18" s="58"/>
       <c r="K18" s="56"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="33" t="s">
         <v>31</v>
@@ -3115,22 +3115,22 @@
       <c r="F19" s="21"/>
       <c r="G19" s="23">
         <f>SUM(G16:G18)</f>
-        <v>5.38</v>
+        <v>10.254591405059433</v>
       </c>
       <c r="H19" s="22" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="23">
-        <f>5476.83*1.15</f>
-        <v>6298.3544999999995</v>
+        <f>4465.4*1.15</f>
+        <v>5135.2099999999991</v>
       </c>
       <c r="J19" s="36">
         <f>G19*I19</f>
-        <v>33885.147209999996</v>
+        <v>52659.48032917524</v>
       </c>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="28"/>
       <c r="C20" s="19"/>
@@ -3143,7 +3143,7 @@
       <c r="J20" s="30"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="37" t="s">
         <v>16</v>
@@ -3157,11 +3157,11 @@
       <c r="I21" s="36"/>
       <c r="J21" s="36">
         <f>SUM(J9:J20)</f>
-        <v>46326.255556332209</v>
+        <v>65100.588675507453</v>
       </c>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="46"/>
       <c r="B22" s="49"/>
       <c r="C22" s="50"/>
@@ -3174,16 +3174,16 @@
       <c r="J22" s="48"/>
       <c r="K22" s="45"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
       <c r="B23" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="76">
+      <c r="C23" s="74">
         <f>J21</f>
-        <v>46326.255556332209</v>
-      </c>
-      <c r="D23" s="76"/>
+        <v>65100.588675507453</v>
+      </c>
+      <c r="D23" s="74"/>
       <c r="E23" s="40"/>
       <c r="F23" s="41"/>
       <c r="G23" s="40"/>
@@ -3191,16 +3191,16 @@
       <c r="I23" s="43"/>
       <c r="J23" s="44"/>
     </row>
-    <row r="24" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="45"/>
       <c r="B24" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="76">
+      <c r="C24" s="74">
         <f>0.13*C23</f>
-        <v>6022.4132223231873</v>
-      </c>
-      <c r="D24" s="76"/>
+        <v>8463.0765278159688</v>
+      </c>
+      <c r="D24" s="74"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45"/>
       <c r="G24" s="45"/>
@@ -3208,85 +3208,85 @@
       <c r="I24" s="45"/>
       <c r="J24" s="45"/>
     </row>
-    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="76">
+      <c r="C25" s="74">
         <f>SUM(C23:D24)</f>
-        <v>52348.668778655396</v>
-      </c>
-      <c r="D25" s="76"/>
-    </row>
-    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>73563.665203323428</v>
+      </c>
+      <c r="D25" s="74"/>
+    </row>
+    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
@@ -3300,25 +3300,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="J1" s="77"/>
       <c r="K1" s="77"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
@@ -3348,7 +3348,7 @@
       <c r="J2" s="78"/>
       <c r="K2" s="78"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="J4" s="79"/>
       <c r="K4" s="79"/>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
         <v>53</v>
       </c>
@@ -3393,7 +3393,7 @@
       <c r="J5" s="80"/>
       <c r="K5" s="80"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="81" t="s">
         <v>47</v>
       </c>
@@ -3409,15 +3409,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="3"/>
       <c r="I7" s="73"/>
       <c r="J7" s="73"/>
@@ -3425,7 +3425,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="M8" s="31"/>
     </row>
-    <row r="9" spans="1:13" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -3489,7 +3489,7 @@
       <c r="K9" s="21"/>
       <c r="M9" s="70"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="55"/>
       <c r="B10" s="59" t="s">
         <v>43</v>
@@ -3518,7 +3518,7 @@
       <c r="K10" s="56"/>
       <c r="M10" s="70"/>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="55"/>
       <c r="B11" s="59" t="s">
         <v>42</v>
@@ -3547,7 +3547,7 @@
       <c r="K11" s="56"/>
       <c r="M11" s="61"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="55"/>
       <c r="B12" s="59" t="s">
         <v>41</v>
@@ -3575,7 +3575,7 @@
       <c r="J12" s="58"/>
       <c r="K12" s="56"/>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="33" t="s">
         <v>31</v>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="33"/>
       <c r="C14" s="19"/>
@@ -3613,7 +3613,7 @@
       <c r="J14" s="36"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -3630,7 +3630,7 @@
       <c r="J15" s="30"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="55"/>
       <c r="B16" s="59" t="s">
         <v>44</v>
@@ -3647,21 +3647,21 @@
         <v>1.8</v>
       </c>
       <c r="G16" s="60">
-        <f>F16</f>
-        <v>1.8</v>
+        <f>PRODUCT(C16:F16)</f>
+        <v>10.012191405059433</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
       <c r="J16" s="58"/>
       <c r="K16" s="56"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="55"/>
       <c r="B17" s="59" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D17" s="12">
         <v>0.874</v>
@@ -3671,15 +3671,15 @@
         <v>1.8</v>
       </c>
       <c r="G17" s="60">
-        <f t="shared" ref="G17:G18" si="2">F17</f>
-        <v>1.8</v>
+        <f t="shared" ref="G17:G18" si="2">PRODUCT(C17:F17)</f>
+        <v>-1.5731999999999999</v>
       </c>
       <c r="H17" s="58"/>
       <c r="I17" s="58"/>
       <c r="J17" s="58"/>
       <c r="K17" s="56"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55"/>
       <c r="B18" s="59" t="s">
         <v>46</v>
@@ -3696,14 +3696,14 @@
       </c>
       <c r="G18" s="60">
         <f t="shared" si="2"/>
-        <v>1.78</v>
+        <v>1.8156000000000001</v>
       </c>
       <c r="H18" s="58"/>
       <c r="I18" s="58"/>
       <c r="J18" s="58"/>
       <c r="K18" s="56"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="33" t="s">
         <v>31</v>
@@ -3714,7 +3714,7 @@
       <c r="F19" s="21"/>
       <c r="G19" s="23">
         <f>SUM(G16:G18)</f>
-        <v>5.38</v>
+        <v>10.254591405059433</v>
       </c>
       <c r="H19" s="22" t="s">
         <v>33</v>
@@ -3724,11 +3724,11 @@
       </c>
       <c r="J19" s="36">
         <f>G19*I19</f>
-        <v>24023.851999999999</v>
+        <v>45790.85246015239</v>
       </c>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="28"/>
       <c r="C20" s="19"/>
@@ -3741,7 +3741,7 @@
       <c r="J20" s="30"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="37" t="s">
         <v>17</v>
@@ -3755,11 +3755,11 @@
       <c r="I21" s="36"/>
       <c r="J21" s="36">
         <f>SUM(J9:J20)</f>
-        <v>34842.207083767142</v>
+        <v>56609.207543919532</v>
       </c>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="46"/>
       <c r="B22" s="49"/>
       <c r="C22" s="50"/>
@@ -3772,7 +3772,7 @@
       <c r="J22" s="48"/>
       <c r="K22" s="45"/>
     </row>
-    <row r="23" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="45"/>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
@@ -3785,62 +3785,62 @@
       <c r="J23" s="45"/>
       <c r="K23" s="45"/>
     </row>
-    <row r="24" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A7:F7"/>

</xml_diff>